<commit_message>
publish PIXm 3.0.2 (using new go-publish, which also fixedup other stuff)
</commit_message>
<xml_diff>
--- a/ITI/PIXm/StructureDefinition-IHE.PIXm.Feed.Audit.Manager.xlsx
+++ b/ITI/PIXm/StructureDefinition-IHE.PIXm.Feed.Audit.Manager.xlsx
@@ -27,13 +27,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://profiles.ihe.net/ITI/PIXm/StructureDefinition/IHE.PIXm.Feed.Audit.Manager</t>
+    <t>https://profiles.ihe.net/ITI/PIXm/StructureDefinition/IHE.PIXm.Feed.Audit.Manager</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-11-08T19:38:05-06:00</t>
+    <t>2022-02-25T14:21:18-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>